<commit_message>
Zápis pokračování do Gantt, úprava struktury Statnice.md
</commit_message>
<xml_diff>
--- a/Státní závěrečné zkoušky/Otázky/Gantt.xlsx
+++ b/Státní závěrečné zkoušky/Otázky/Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ef484bc4f40e753/Bakalářská práce/Státní závěrečné zkoušky/Otázky/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{73A8C43E-3182-8447-A6C7-CC7D48974769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{739641E2-B384-C941-8876-75D552BACAB8}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{73A8C43E-3182-8447-A6C7-CC7D48974769}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF2B5A9E-A096-C64E-A708-B57714726BDA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19820" activeTab="1" xr2:uid="{196274B7-E9B6-054A-946B-71D9237123A5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19820" xr2:uid="{196274B7-E9B6-054A-946B-71D9237123A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -360,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -430,6 +430,7 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475068D2-3FCF-C848-8C20-861F3B0DA572}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -890,6 +891,9 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="25">
+        <v>0.16650000000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
@@ -1376,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA571D2-B30F-6044-AFAE-E5DB9529F9D8}">
   <dimension ref="A1:BX41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2218,7 +2222,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="19">
         <f>Sheet1!E3</f>
-        <v>0</v>
+        <v>0.16650000000000001</v>
       </c>
       <c r="D8" s="18">
         <f>Sheet1!B3</f>

</xml_diff>